<commit_message>
more statistics and a seuquence diagram documentation
</commit_message>
<xml_diff>
--- a/result/results.xlsx
+++ b/result/results.xlsx
@@ -1,31 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dados\0Code\textureSSD\result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{834A0CB7-808C-401A-8969-C43E8DF0BBC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6924D0-2C5B-4825-A2DD-97AC0684A177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="28800" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="90">
   <si>
     <t xml:space="preserve">      MSE</t>
   </si>
@@ -262,6 +272,39 @@
   </si>
   <si>
     <t>0bdd44d530 - Images: 4</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>std</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>time_sec</t>
+  </si>
+  <si>
+    <t>mse</t>
+  </si>
+  <si>
+    <t>dssim</t>
+  </si>
+  <si>
+    <t>lbp_distance</t>
   </si>
 </sst>
 </file>
@@ -620,7 +663,18 @@
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -637,16 +691,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>188746</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>160171</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -669,7 +723,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7172325" y="1141246"/>
+          <a:off x="7905750" y="1312696"/>
           <a:ext cx="9934575" cy="4954754"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -682,15 +736,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>342265</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>13970</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>245082</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -713,8 +767,233 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9715500" y="7191375"/>
-          <a:ext cx="4066540" cy="3061970"/>
+          <a:off x="10506075" y="6877050"/>
+          <a:ext cx="5464782" cy="4114800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07F81942-DAD5-DF0A-2992-05C8F066CA64}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="504825" y="990600"/>
+          <a:ext cx="11325225" cy="5648325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>10384</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>86052</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD8C3B27-36E0-1CDE-ED91-1C123B17FBA6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12144375" y="981075"/>
+          <a:ext cx="6154009" cy="2343477"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagem 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FCD8E09-31E2-6F9E-ED94-9639452080B0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="590550" y="6877050"/>
+          <a:ext cx="11334750" cy="5648325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagem 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5A55D24-34E8-1928-F3CF-96ED157C0D43}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="666750" y="12858750"/>
+          <a:ext cx="11334750" cy="5648325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>129</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagem 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E35826FE-6512-2B95-47A8-4F446B31188D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="695325" y="19088100"/>
+          <a:ext cx="11325225" cy="5648325"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -991,14 +1270,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11:J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
     <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
     <col min="10" max="10" width="10.85546875" customWidth="1"/>
@@ -1912,4 +2192,1051 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A5A7372-7366-4E8A-A7B1-CFFB77B17071}">
+  <dimension ref="U21:AD119"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AC116" sqref="AC116:AC119"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="21" spans="21:29" x14ac:dyDescent="0.25">
+      <c r="V21" t="s">
+        <v>79</v>
+      </c>
+      <c r="W21" t="s">
+        <v>69</v>
+      </c>
+      <c r="X21" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="21:29" x14ac:dyDescent="0.25">
+      <c r="U22" t="s">
+        <v>86</v>
+      </c>
+      <c r="V22">
+        <v>16.229949999999999</v>
+      </c>
+      <c r="W22">
+        <v>19.391649000000001</v>
+      </c>
+      <c r="X22">
+        <v>20.621970999999998</v>
+      </c>
+      <c r="Y22">
+        <v>24.921181000000001</v>
+      </c>
+      <c r="Z22">
+        <v>27.695557999999998</v>
+      </c>
+      <c r="AA22">
+        <v>21.590599000000001</v>
+      </c>
+      <c r="AB22">
+        <v>3.333202</v>
+      </c>
+      <c r="AC22">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="23" spans="21:29" x14ac:dyDescent="0.25">
+      <c r="U23" t="s">
+        <v>87</v>
+      </c>
+      <c r="V23">
+        <v>511.83060499999999</v>
+      </c>
+      <c r="W23">
+        <v>681.30477399999995</v>
+      </c>
+      <c r="X23">
+        <v>857.39721599999996</v>
+      </c>
+      <c r="Y23">
+        <v>1051.18454</v>
+      </c>
+      <c r="Z23">
+        <v>1231.950789</v>
+      </c>
+      <c r="AA23">
+        <v>848.56772899999999</v>
+      </c>
+      <c r="AB23">
+        <v>216.6223</v>
+      </c>
+      <c r="AC23">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="24" spans="21:29" x14ac:dyDescent="0.25">
+      <c r="U24" t="s">
+        <v>88</v>
+      </c>
+      <c r="V24">
+        <v>0.22789400000000001</v>
+      </c>
+      <c r="W24">
+        <v>0.26556400000000002</v>
+      </c>
+      <c r="X24">
+        <v>0.27986800000000001</v>
+      </c>
+      <c r="Y24">
+        <v>0.292379</v>
+      </c>
+      <c r="Z24">
+        <v>0.38566499999999998</v>
+      </c>
+      <c r="AA24">
+        <v>0.28378999999999999</v>
+      </c>
+      <c r="AB24">
+        <v>3.4841999999999998E-2</v>
+      </c>
+      <c r="AC24">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="25" spans="21:29" x14ac:dyDescent="0.25">
+      <c r="U25" t="s">
+        <v>89</v>
+      </c>
+      <c r="V25">
+        <v>4.4221999999999997E-2</v>
+      </c>
+      <c r="W25">
+        <v>9.2244000000000007E-2</v>
+      </c>
+      <c r="X25">
+        <v>0.14713499999999999</v>
+      </c>
+      <c r="Y25">
+        <v>0.217193</v>
+      </c>
+      <c r="Z25">
+        <v>0.39388099999999998</v>
+      </c>
+      <c r="AA25">
+        <v>0.155749</v>
+      </c>
+      <c r="AB25">
+        <v>6.9389999999999993E-2</v>
+      </c>
+      <c r="AC25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="29" spans="21:29" x14ac:dyDescent="0.25">
+      <c r="V29" t="s">
+        <v>79</v>
+      </c>
+      <c r="W29" t="s">
+        <v>69</v>
+      </c>
+      <c r="X29" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC29" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="21:29" x14ac:dyDescent="0.25">
+      <c r="U30" t="s">
+        <v>86</v>
+      </c>
+      <c r="V30">
+        <v>16.229949999999999</v>
+      </c>
+      <c r="W30">
+        <v>19.511531000000002</v>
+      </c>
+      <c r="X30">
+        <v>21.707916000000001</v>
+      </c>
+      <c r="Y30">
+        <v>25.981622000000002</v>
+      </c>
+      <c r="Z30">
+        <v>40116.067750000002</v>
+      </c>
+      <c r="AA30">
+        <v>171.71351200000001</v>
+      </c>
+      <c r="AB30">
+        <v>2393.8204479999999</v>
+      </c>
+      <c r="AC30">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="31" spans="21:29" x14ac:dyDescent="0.25">
+      <c r="U31" t="s">
+        <v>87</v>
+      </c>
+      <c r="V31">
+        <v>511.83060499999999</v>
+      </c>
+      <c r="W31">
+        <v>701.53475100000003</v>
+      </c>
+      <c r="X31">
+        <v>869.39398100000005</v>
+      </c>
+      <c r="Y31">
+        <v>1055.1171449999999</v>
+      </c>
+      <c r="Z31">
+        <v>1231.950789</v>
+      </c>
+      <c r="AA31">
+        <v>862.52281700000003</v>
+      </c>
+      <c r="AB31">
+        <v>211.14699300000001</v>
+      </c>
+      <c r="AC31">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="32" spans="21:29" x14ac:dyDescent="0.25">
+      <c r="U32" t="s">
+        <v>88</v>
+      </c>
+      <c r="V32">
+        <v>0.211394</v>
+      </c>
+      <c r="W32">
+        <v>0.24923999999999999</v>
+      </c>
+      <c r="X32">
+        <v>0.27537299999999998</v>
+      </c>
+      <c r="Y32">
+        <v>0.28977599999999998</v>
+      </c>
+      <c r="Z32">
+        <v>0.38566499999999998</v>
+      </c>
+      <c r="AA32">
+        <v>0.27698200000000001</v>
+      </c>
+      <c r="AB32">
+        <v>3.5763999999999997E-2</v>
+      </c>
+      <c r="AC32">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="33" spans="21:29" x14ac:dyDescent="0.25">
+      <c r="U33" t="s">
+        <v>89</v>
+      </c>
+      <c r="V33">
+        <v>4.4221999999999997E-2</v>
+      </c>
+      <c r="W33">
+        <v>9.8294000000000006E-2</v>
+      </c>
+      <c r="X33">
+        <v>0.16867499999999999</v>
+      </c>
+      <c r="Y33">
+        <v>0.23413400000000001</v>
+      </c>
+      <c r="Z33">
+        <v>0.39388099999999998</v>
+      </c>
+      <c r="AA33">
+        <v>0.172543</v>
+      </c>
+      <c r="AB33">
+        <v>7.5604000000000005E-2</v>
+      </c>
+      <c r="AC33">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="37" spans="21:29" x14ac:dyDescent="0.25">
+      <c r="V37" t="s">
+        <v>79</v>
+      </c>
+      <c r="W37" t="s">
+        <v>69</v>
+      </c>
+      <c r="X37" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z37" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA37" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB37" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC37" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="21:29" x14ac:dyDescent="0.25">
+      <c r="U38" t="s">
+        <v>86</v>
+      </c>
+      <c r="V38">
+        <f>V30-V22</f>
+        <v>0</v>
+      </c>
+      <c r="W38">
+        <f t="shared" ref="W38:AC38" si="0">W30-W22</f>
+        <v>0.11988200000000049</v>
+      </c>
+      <c r="X38">
+        <f t="shared" si="0"/>
+        <v>1.0859450000000024</v>
+      </c>
+      <c r="Y38">
+        <f t="shared" si="0"/>
+        <v>1.0604410000000009</v>
+      </c>
+      <c r="Z38">
+        <f t="shared" si="0"/>
+        <v>40088.372192000003</v>
+      </c>
+      <c r="AA38">
+        <f t="shared" si="0"/>
+        <v>150.12291300000001</v>
+      </c>
+      <c r="AB38">
+        <f t="shared" si="0"/>
+        <v>2390.4872460000001</v>
+      </c>
+      <c r="AC38">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="21:29" x14ac:dyDescent="0.25">
+      <c r="U39" t="s">
+        <v>87</v>
+      </c>
+      <c r="V39">
+        <f t="shared" ref="V39:AC41" si="1">V31-V23</f>
+        <v>0</v>
+      </c>
+      <c r="W39">
+        <f t="shared" si="1"/>
+        <v>20.229977000000076</v>
+      </c>
+      <c r="X39">
+        <f t="shared" si="1"/>
+        <v>11.996765000000096</v>
+      </c>
+      <c r="Y39">
+        <f t="shared" si="1"/>
+        <v>3.9326049999999668</v>
+      </c>
+      <c r="Z39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AA39">
+        <f t="shared" si="1"/>
+        <v>13.955088000000046</v>
+      </c>
+      <c r="AB39">
+        <f t="shared" si="1"/>
+        <v>-5.4753069999999866</v>
+      </c>
+      <c r="AC39">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="21:29" x14ac:dyDescent="0.25">
+      <c r="U40" t="s">
+        <v>88</v>
+      </c>
+      <c r="V40">
+        <f>V32-V24</f>
+        <v>-1.6500000000000015E-2</v>
+      </c>
+      <c r="W40">
+        <f t="shared" si="1"/>
+        <v>-1.6324000000000033E-2</v>
+      </c>
+      <c r="X40">
+        <f t="shared" si="1"/>
+        <v>-4.4950000000000268E-3</v>
+      </c>
+      <c r="Y40">
+        <f t="shared" si="1"/>
+        <v>-2.603000000000022E-3</v>
+      </c>
+      <c r="Z40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AA40">
+        <f t="shared" si="1"/>
+        <v>-6.8079999999999807E-3</v>
+      </c>
+      <c r="AB40">
+        <f t="shared" si="1"/>
+        <v>9.2199999999999921E-4</v>
+      </c>
+      <c r="AC40">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="21:29" x14ac:dyDescent="0.25">
+      <c r="U41" t="s">
+        <v>89</v>
+      </c>
+      <c r="V41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W41">
+        <f t="shared" si="1"/>
+        <v>6.0499999999999998E-3</v>
+      </c>
+      <c r="X41">
+        <f t="shared" si="1"/>
+        <v>2.1540000000000004E-2</v>
+      </c>
+      <c r="Y41">
+        <f t="shared" si="1"/>
+        <v>1.6941000000000012E-2</v>
+      </c>
+      <c r="Z41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AA41">
+        <f t="shared" si="1"/>
+        <v>1.6794000000000003E-2</v>
+      </c>
+      <c r="AB41">
+        <f t="shared" si="1"/>
+        <v>6.2140000000000112E-3</v>
+      </c>
+      <c r="AC41">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="77" spans="22:30" x14ac:dyDescent="0.25">
+      <c r="W77" t="s">
+        <v>79</v>
+      </c>
+      <c r="X77" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y77" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z77" t="s">
+        <v>81</v>
+      </c>
+      <c r="AA77" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB77" t="s">
+        <v>83</v>
+      </c>
+      <c r="AC77" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD77" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="78" spans="22:30" x14ac:dyDescent="0.25">
+      <c r="V78" t="s">
+        <v>86</v>
+      </c>
+      <c r="W78">
+        <v>16.229949999999999</v>
+      </c>
+      <c r="X78">
+        <v>19.694673000000002</v>
+      </c>
+      <c r="Y78">
+        <v>24.653563999999999</v>
+      </c>
+      <c r="Z78">
+        <v>27.876825</v>
+      </c>
+      <c r="AA78">
+        <v>41923.755803</v>
+      </c>
+      <c r="AB78">
+        <v>278.71281099999999</v>
+      </c>
+      <c r="AC78">
+        <v>3183.6555760000001</v>
+      </c>
+      <c r="AD78">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="79" spans="22:30" x14ac:dyDescent="0.25">
+      <c r="V79" t="s">
+        <v>87</v>
+      </c>
+      <c r="W79">
+        <v>511.83060499999999</v>
+      </c>
+      <c r="X79">
+        <v>720.81045900000004</v>
+      </c>
+      <c r="Y79">
+        <v>879.03499699999998</v>
+      </c>
+      <c r="Z79">
+        <v>1050.566317</v>
+      </c>
+      <c r="AA79">
+        <v>1298.5764140000001</v>
+      </c>
+      <c r="AB79">
+        <v>873.73495800000001</v>
+      </c>
+      <c r="AC79">
+        <v>203.455186</v>
+      </c>
+      <c r="AD79">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="80" spans="22:30" x14ac:dyDescent="0.25">
+      <c r="V80" t="s">
+        <v>88</v>
+      </c>
+      <c r="W80">
+        <v>0.19650200000000001</v>
+      </c>
+      <c r="X80">
+        <v>0.238311</v>
+      </c>
+      <c r="Y80">
+        <v>0.27006400000000003</v>
+      </c>
+      <c r="Z80">
+        <v>0.28697099999999998</v>
+      </c>
+      <c r="AA80">
+        <v>0.38566499999999998</v>
+      </c>
+      <c r="AB80">
+        <v>0.267816</v>
+      </c>
+      <c r="AC80">
+        <v>3.9704999999999997E-2</v>
+      </c>
+      <c r="AD80">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="81" spans="22:30" x14ac:dyDescent="0.25">
+      <c r="V81" t="s">
+        <v>89</v>
+      </c>
+      <c r="W81">
+        <v>4.4221999999999997E-2</v>
+      </c>
+      <c r="X81">
+        <v>0.116647</v>
+      </c>
+      <c r="Y81">
+        <v>0.168762</v>
+      </c>
+      <c r="Z81">
+        <v>0.22775100000000001</v>
+      </c>
+      <c r="AA81">
+        <v>0.39388099999999998</v>
+      </c>
+      <c r="AB81">
+        <v>0.17299800000000001</v>
+      </c>
+      <c r="AC81">
+        <v>7.1170999999999998E-2</v>
+      </c>
+      <c r="AD81">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="84" spans="22:30" x14ac:dyDescent="0.25">
+      <c r="W84" t="s">
+        <v>79</v>
+      </c>
+      <c r="X84" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y84" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z84" t="s">
+        <v>81</v>
+      </c>
+      <c r="AA84" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB84" t="s">
+        <v>83</v>
+      </c>
+      <c r="AC84" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD84" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="85" spans="22:30" x14ac:dyDescent="0.25">
+      <c r="V85" t="s">
+        <v>86</v>
+      </c>
+      <c r="W85">
+        <f>W78-V30</f>
+        <v>0</v>
+      </c>
+      <c r="X85">
+        <f t="shared" ref="X85:AD85" si="2">X78-W30</f>
+        <v>0.18314200000000014</v>
+      </c>
+      <c r="Y85">
+        <f t="shared" si="2"/>
+        <v>2.9456479999999985</v>
+      </c>
+      <c r="Z85">
+        <f t="shared" si="2"/>
+        <v>1.8952029999999986</v>
+      </c>
+      <c r="AA85">
+        <f t="shared" si="2"/>
+        <v>1807.688052999998</v>
+      </c>
+      <c r="AB85">
+        <f t="shared" si="2"/>
+        <v>106.99929899999998</v>
+      </c>
+      <c r="AC85">
+        <f t="shared" si="2"/>
+        <v>789.83512800000017</v>
+      </c>
+      <c r="AD85">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="86" spans="22:30" x14ac:dyDescent="0.25">
+      <c r="V86" t="s">
+        <v>87</v>
+      </c>
+      <c r="W86">
+        <f t="shared" ref="W86:AD88" si="3">W79-V31</f>
+        <v>0</v>
+      </c>
+      <c r="X86">
+        <f t="shared" si="3"/>
+        <v>19.275708000000009</v>
+      </c>
+      <c r="Y86">
+        <f t="shared" si="3"/>
+        <v>9.6410159999999223</v>
+      </c>
+      <c r="Z86">
+        <f t="shared" si="3"/>
+        <v>-4.5508279999999104</v>
+      </c>
+      <c r="AA86">
+        <f t="shared" si="3"/>
+        <v>66.625625000000127</v>
+      </c>
+      <c r="AB86">
+        <f t="shared" si="3"/>
+        <v>11.212140999999974</v>
+      </c>
+      <c r="AC86">
+        <f t="shared" si="3"/>
+        <v>-7.6918070000000114</v>
+      </c>
+      <c r="AD86">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="87" spans="22:30" x14ac:dyDescent="0.25">
+      <c r="V87" t="s">
+        <v>88</v>
+      </c>
+      <c r="W87">
+        <f>W80-V32</f>
+        <v>-1.4891999999999989E-2</v>
+      </c>
+      <c r="X87">
+        <f t="shared" ref="X87:AD87" si="4">X80-W32</f>
+        <v>-1.0928999999999994E-2</v>
+      </c>
+      <c r="Y87">
+        <f t="shared" si="4"/>
+        <v>-5.3089999999999526E-3</v>
+      </c>
+      <c r="Z87">
+        <f t="shared" si="4"/>
+        <v>-2.8050000000000019E-3</v>
+      </c>
+      <c r="AA87">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AB87">
+        <f t="shared" si="4"/>
+        <v>-9.1660000000000075E-3</v>
+      </c>
+      <c r="AC87">
+        <f t="shared" si="4"/>
+        <v>3.9410000000000001E-3</v>
+      </c>
+      <c r="AD87">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="88" spans="22:30" x14ac:dyDescent="0.25">
+      <c r="V88" t="s">
+        <v>89</v>
+      </c>
+      <c r="W88">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="X88">
+        <f t="shared" si="3"/>
+        <v>1.8352999999999994E-2</v>
+      </c>
+      <c r="Y88">
+        <f t="shared" si="3"/>
+        <v>8.7000000000003741E-5</v>
+      </c>
+      <c r="Z88">
+        <f t="shared" si="3"/>
+        <v>-6.3829999999999998E-3</v>
+      </c>
+      <c r="AA88">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AB88">
+        <f t="shared" si="3"/>
+        <v>4.5500000000001095E-4</v>
+      </c>
+      <c r="AC88">
+        <f t="shared" si="3"/>
+        <v>-4.4330000000000064E-3</v>
+      </c>
+      <c r="AD88">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="106" spans="22:30" x14ac:dyDescent="0.25">
+      <c r="W106" t="s">
+        <v>79</v>
+      </c>
+      <c r="X106" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y106" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z106" t="s">
+        <v>81</v>
+      </c>
+      <c r="AA106" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB106" t="s">
+        <v>83</v>
+      </c>
+      <c r="AC106" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD106" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="107" spans="22:30" x14ac:dyDescent="0.25">
+      <c r="V107" t="s">
+        <v>86</v>
+      </c>
+      <c r="W107">
+        <v>16.229949999999999</v>
+      </c>
+      <c r="X107">
+        <v>20.074041000000001</v>
+      </c>
+      <c r="Y107">
+        <v>24.687047</v>
+      </c>
+      <c r="Z107">
+        <v>28.884568999999999</v>
+      </c>
+      <c r="AA107">
+        <v>41923.755803</v>
+      </c>
+      <c r="AB107">
+        <v>221.21638799999999</v>
+      </c>
+      <c r="AC107">
+        <v>2790.9722809999998</v>
+      </c>
+      <c r="AD107">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="108" spans="22:30" x14ac:dyDescent="0.25">
+      <c r="V108" t="s">
+        <v>87</v>
+      </c>
+      <c r="W108">
+        <v>406.68885399999999</v>
+      </c>
+      <c r="X108">
+        <v>673.52833099999998</v>
+      </c>
+      <c r="Y108">
+        <v>835.96323900000004</v>
+      </c>
+      <c r="Z108">
+        <v>998.14219200000002</v>
+      </c>
+      <c r="AA108">
+        <v>1298.5764140000001</v>
+      </c>
+      <c r="AB108">
+        <v>827.91720399999997</v>
+      </c>
+      <c r="AC108">
+        <v>212.97742299999999</v>
+      </c>
+      <c r="AD108">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="109" spans="22:30" x14ac:dyDescent="0.25">
+      <c r="V109" t="s">
+        <v>88</v>
+      </c>
+      <c r="W109">
+        <v>0.16550300000000001</v>
+      </c>
+      <c r="X109">
+        <v>0.21665499999999999</v>
+      </c>
+      <c r="Y109">
+        <v>0.246948</v>
+      </c>
+      <c r="Z109">
+        <v>0.28173399999999998</v>
+      </c>
+      <c r="AA109">
+        <v>0.38566499999999998</v>
+      </c>
+      <c r="AB109">
+        <v>0.25374400000000003</v>
+      </c>
+      <c r="AC109">
+        <v>4.3712000000000001E-2</v>
+      </c>
+      <c r="AD109">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="110" spans="22:30" x14ac:dyDescent="0.25">
+      <c r="V110" t="s">
+        <v>89</v>
+      </c>
+      <c r="W110">
+        <v>4.4221999999999997E-2</v>
+      </c>
+      <c r="X110">
+        <v>0.11469500000000001</v>
+      </c>
+      <c r="Y110">
+        <v>0.169541</v>
+      </c>
+      <c r="Z110">
+        <v>0.23721100000000001</v>
+      </c>
+      <c r="AA110">
+        <v>0.39388099999999998</v>
+      </c>
+      <c r="AB110">
+        <v>0.176228</v>
+      </c>
+      <c r="AC110">
+        <v>7.2464000000000001E-2</v>
+      </c>
+      <c r="AD110">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="115" spans="22:30" x14ac:dyDescent="0.25">
+      <c r="W115" t="s">
+        <v>79</v>
+      </c>
+      <c r="X115" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y115" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z115" t="s">
+        <v>81</v>
+      </c>
+      <c r="AA115" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB115" t="s">
+        <v>83</v>
+      </c>
+      <c r="AC115" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD115" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="116" spans="22:30" x14ac:dyDescent="0.25">
+      <c r="V116" t="s">
+        <v>86</v>
+      </c>
+      <c r="W116">
+        <f>W107-W78</f>
+        <v>0</v>
+      </c>
+      <c r="Y116">
+        <f>Y107-Y78</f>
+        <v>3.3483000000000374E-2</v>
+      </c>
+      <c r="AB116">
+        <f>AB107-AB78</f>
+        <v>-57.496422999999993</v>
+      </c>
+      <c r="AC116">
+        <f>AC107-AC78</f>
+        <v>-392.68329500000027</v>
+      </c>
+    </row>
+    <row r="117" spans="22:30" x14ac:dyDescent="0.25">
+      <c r="V117" t="s">
+        <v>87</v>
+      </c>
+      <c r="W117">
+        <f t="shared" ref="W117:Y119" si="5">W108-W79</f>
+        <v>-105.141751</v>
+      </c>
+      <c r="Y117">
+        <f t="shared" si="5"/>
+        <v>-43.071757999999932</v>
+      </c>
+      <c r="AB117">
+        <f t="shared" ref="AB117:AC117" si="6">AB108-AB79</f>
+        <v>-45.817754000000036</v>
+      </c>
+      <c r="AC117">
+        <f t="shared" si="6"/>
+        <v>9.5222369999999898</v>
+      </c>
+    </row>
+    <row r="118" spans="22:30" x14ac:dyDescent="0.25">
+      <c r="V118" t="s">
+        <v>88</v>
+      </c>
+      <c r="W118">
+        <f t="shared" si="5"/>
+        <v>-3.0998999999999999E-2</v>
+      </c>
+      <c r="Y118">
+        <f t="shared" si="5"/>
+        <v>-2.3116000000000025E-2</v>
+      </c>
+      <c r="AB118">
+        <f t="shared" ref="AB118:AC118" si="7">AB109-AB80</f>
+        <v>-1.4071999999999973E-2</v>
+      </c>
+      <c r="AC118">
+        <f t="shared" si="7"/>
+        <v>4.0070000000000036E-3</v>
+      </c>
+    </row>
+    <row r="119" spans="22:30" x14ac:dyDescent="0.25">
+      <c r="V119" t="s">
+        <v>89</v>
+      </c>
+      <c r="W119">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Y119">
+        <f t="shared" si="5"/>
+        <v>7.7900000000000191E-4</v>
+      </c>
+      <c r="AB119">
+        <f t="shared" ref="AB119:AC119" si="8">AB110-AB81</f>
+        <v>3.2299999999999829E-3</v>
+      </c>
+      <c r="AC119">
+        <f t="shared" si="8"/>
+        <v>1.2930000000000025E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="W85:AC88">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>